<commit_message>
add epsg to area polygon import
</commit_message>
<xml_diff>
--- a/tests/edb/data/areasourceactivities.xlsx
+++ b/tests/edb/data/areasourceactivities.xlsx
@@ -78,7 +78,7 @@
     <t xml:space="preserve">vedspis1</t>
   </si>
   <si>
-    <t xml:space="preserve">source1</t>
+    <t xml:space="preserve">areasource1</t>
   </si>
   <si>
     <t xml:space="preserve">POLYGON ((2449702.70275976 5078151.62902639,2450837.61057971 5078021.39370279,2450744.58534857 5077216.7254534,2450102.71125368 5077077.18760669,2449591.07248239 5077249.2842843,2449702.70275976 5078151.62902639))</t>
@@ -93,7 +93,7 @@
     <t xml:space="preserve">vedspis2</t>
   </si>
   <si>
-    <t xml:space="preserve">source2</t>
+    <t xml:space="preserve">areasource2</t>
   </si>
   <si>
     <t xml:space="preserve">POLYGON ((2449418.97580478 5076253.91431107,2449879.45069894 5076691.13289745,2450521.32479382 5076737.64551302,2450814.35427192 5076374.84711156,2450698.072733 5075681.80913954,2449651.53888264 5075328.3132612,2449418.97580478 5076253.91431107))</t>
@@ -105,7 +105,7 @@
     <t xml:space="preserve">facility2</t>
   </si>
   <si>
-    <t xml:space="preserve">source3</t>
+    <t xml:space="preserve">areasource3</t>
   </si>
   <si>
     <t xml:space="preserve">POLYGON ((2441769.48069413 5078251.37652748,2442293.71664687 5078431.58263624,2442739.3172067 5078185.84703339,2442880.205619 5078212.05883103,2443948.3363727 5076603.30975106,2442788.46432727 5076478.80371229,2441769.48069413 5078251.37652748))</t>
@@ -120,7 +120,7 @@
     <t xml:space="preserve">pellet1</t>
   </si>
   <si>
-    <t xml:space="preserve">source4</t>
+    <t xml:space="preserve">areasource4</t>
   </si>
   <si>
     <t xml:space="preserve">POLYGON ((2445081.11344401 5079793.39383044,2447785.96016067 5080725.2070534,2447617.71610652 5077813.29073163,2445301.12489943 5078033.30218706,2445081.11344401 5079793.39383044))</t>
@@ -556,10 +556,10 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.09"/>
@@ -666,7 +666,9 @@
       <c r="D3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="n">
+        <v>3857</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
         <v>19</v>
@@ -702,7 +704,9 @@
       <c r="D4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="n">
+        <v>3857</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>28</v>
       </c>
@@ -739,7 +743,9 @@
       <c r="D5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="n">
+        <v>3857</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>19</v>
       </c>
@@ -818,7 +824,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
   </cols>
@@ -870,7 +876,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
@@ -990,7 +996,7 @@
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -2484,7 +2490,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
@@ -2547,7 +2553,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>

</xml_diff>

<commit_message>
import several activities per point or area
</commit_message>
<xml_diff>
--- a/tests/edb/data/areasourceactivities.xlsx
+++ b/tests/edb/data/areasourceactivities.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="114">
   <si>
     <t xml:space="preserve">facility_id</t>
   </si>
@@ -66,75 +66,72 @@
     <t xml:space="preserve">unit</t>
   </si>
   <si>
+    <t xml:space="preserve">act:Residential-plants-Open-fireplaces-wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vedspis1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">areasource1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLYGON ((2449702.70275976 5078151.62902639,2450837.61057971 5078021.39370279,2450744.58534857 5077216.7254534,2450102.71125368 5077077.18760669,2449591.07248239 5077249.2842843,2449702.70275976 5078151.62902639))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vedspis2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">areasource2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLYGON ((2449418.97580478 5076253.91431107,2449879.45069894 5076691.13289745,2450521.32479382 5076737.64551302,2450814.35427192 5076374.84711156,2450698.072733 5075681.80913954,2449651.53888264 5075328.3132612,2449418.97580478 5076253.91431107))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">areasource3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLYGON ((2441769.48069413 5078251.37652748,2442293.71664687 5078431.58263624,2442739.3172067 5078185.84703339,2442880.205619 5078212.05883103,2443948.3363727 5076603.30975106,2442788.46432727 5076478.80371229,2441769.48069413 5078251.37652748))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">officehours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ton/year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pellet1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">areasource4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLYGON ((2445081.11344401 5079793.39383044,2447785.96016067 5080725.2070534,2447617.71610652 5077813.29073163,2445301.12489943 5078033.30218706,2445081.11344401 5079793.39383044))</t>
+  </si>
+  <si>
     <t xml:space="preserve">activity_name</t>
   </si>
   <si>
-    <t xml:space="preserve">activity_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activity_unit (do not fill in, automatically taken from activity-sheet)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vedspis1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">areasource1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POLYGON ((2449702.70275976 5078151.62902639,2450837.61057971 5078021.39370279,2450744.58534857 5077216.7254534,2450102.71125368 5077077.18760669,2449591.07248239 5077249.2842843,2449702.70275976 5078151.62902639))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3</t>
+    <t xml:space="preserve">activity_unit</t>
   </si>
   <si>
     <t xml:space="preserve">Residential-plants-Open-fireplaces-wood</t>
   </si>
   <si>
-    <t xml:space="preserve">vedspis2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">areasource2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POLYGON ((2449418.97580478 5076253.91431107,2449879.45069894 5076691.13289745,2450521.32479382 5076737.64551302,2450814.35427192 5076374.84711156,2450698.072733 5075681.80913954,2449651.53888264 5075328.3132612,2449418.97580478 5076253.91431107))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">areasource3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POLYGON ((2441769.48069413 5078251.37652748,2442293.71664687 5078431.58263624,2442739.3172067 5078185.84703339,2442880.205619 5078212.05883103,2443948.3363727 5076603.30975106,2442788.46432727 5076478.80371229,2441769.48069413 5078251.37652748))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">officehours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ton/year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pellet1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">areasource4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POLYGON ((2445081.11344401 5079793.39383044,2447785.96016067 5080725.2070534,2447617.71610652 5077813.29073163,2445301.12489943 5078033.30218706,2445081.11344401 5079793.39383044))</t>
+    <t xml:space="preserve">GJ/yr</t>
   </si>
   <si>
     <t xml:space="preserve">Residential-plants-pellet-stove-pellet</t>
   </si>
   <si>
-    <t xml:space="preserve">activity_unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GJ/yr</t>
-  </si>
-  <si>
     <t xml:space="preserve">m3/yr</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t xml:space="preserve">emissionfactor_unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activity_unit (do not fill in, automatically taken from activity-sheet to check compatibility of units)</t>
   </si>
   <si>
     <t xml:space="preserve">CO</t>
@@ -464,11 +464,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -553,19 +553,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="34.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="34.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -611,67 +612,54 @@
       <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>3857</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="N2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="0" t="n">
+      <c r="N2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="P2" s="2" t="str">
-        <f aca="false">IF(ISBLANK(N2),"",INDEX(Activity!B:B,MATCH(N2,Activity!A:A,0),1))</f>
-        <v>GJ/yr</v>
-      </c>
-      <c r="Q2" s="1"/>
+      <c r="O2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>3857</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -679,39 +667,32 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="0" t="n">
+      <c r="N3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="P3" s="2" t="str">
-        <f aca="false">IF(ISBLANK(N3),"",INDEX(Activity!B:B,MATCH(N3,Activity!A:A,0),1))</f>
-        <v>GJ/yr</v>
-      </c>
-      <c r="Q3" s="1"/>
+      <c r="O3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>3857</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -721,47 +702,36 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="2" t="str">
-        <f aca="false">IF(ISBLANK(N4),"",INDEX(Activity!B:B,MATCH(N4,Activity!A:A,0),1))</f>
-        <v/>
-      </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>3857</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="N5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" s="0" t="n">
+      <c r="N5" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="P5" s="2" t="str">
-        <f aca="false">IF(ISBLANK(N5),"",INDEX(Activity!B:B,MATCH(N5,Activity!A:A,0),1))</f>
-        <v>m3/yr</v>
-      </c>
-      <c r="Q5" s="1"/>
+      <c r="O5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
@@ -779,9 +749,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
+      <c r="P6" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
@@ -796,11 +764,9 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
+      <c r="T8" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -824,34 +790,34 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>34</v>
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -873,35 +839,35 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>40</v>
@@ -912,14 +878,14 @@
       <c r="D2" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="2" t="str">
+      <c r="E2" s="3" t="str">
         <f aca="false">INDEX(Activity!B:B,MATCH(A2,Activity!A:A,0),1)</f>
         <v>GJ/yr</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>42</v>
@@ -930,14 +896,14 @@
       <c r="D3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="2" t="str">
+      <c r="E3" s="3" t="str">
         <f aca="false">INDEX(Activity!B:B,MATCH(A3,Activity!A:A,0),1)</f>
         <v>GJ/yr</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>43</v>
@@ -948,14 +914,14 @@
       <c r="D4" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="2" t="str">
+      <c r="E4" s="3" t="str">
         <f aca="false">INDEX(Activity!B:B,MATCH(A4,Activity!A:A,0),1)</f>
         <v>GJ/yr</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>43</v>
@@ -966,7 +932,7 @@
       <c r="D5" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="2" t="str">
+      <c r="E5" s="3" t="str">
         <f aca="false">INDEX(Activity!B:B,MATCH(A5,Activity!A:A,0),1)</f>
         <v>m3/yr</v>
       </c>
@@ -996,34 +962,34 @@
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1031,7 +997,7 @@
       <c r="A2" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -1057,7 +1023,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -1083,7 +1049,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -1109,7 +1075,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -1135,7 +1101,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -1161,7 +1127,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -1187,7 +1153,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -1213,7 +1179,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -1239,7 +1205,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -1265,7 +1231,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -1291,7 +1257,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -1317,7 +1283,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C13" s="0" t="n">
@@ -1343,7 +1309,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -1369,7 +1335,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -1395,7 +1361,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -1421,7 +1387,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C17" s="0" t="n">
@@ -1447,7 +1413,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -1473,7 +1439,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -1499,7 +1465,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -1525,7 +1491,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C21" s="0" t="n">
@@ -1551,7 +1517,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C22" s="0" t="n">
@@ -1577,7 +1543,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -1603,7 +1569,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -1629,7 +1595,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -1655,43 +1621,43 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="J26" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="K26" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="L26" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="M26" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="N26" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1734,39 +1700,39 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I28" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="0" t="n">
@@ -1792,7 +1758,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -1818,7 +1784,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -1844,7 +1810,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C32" s="0" t="n">
@@ -1870,7 +1836,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C33" s="0" t="n">
@@ -1896,7 +1862,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C34" s="0" t="n">
@@ -1922,7 +1888,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C35" s="0" t="n">
@@ -1948,7 +1914,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C36" s="0" t="n">
@@ -1974,7 +1940,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C37" s="0" t="n">
@@ -2000,7 +1966,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C38" s="0" t="n">
@@ -2026,7 +1992,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C39" s="0" t="n">
@@ -2052,7 +2018,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C40" s="0" t="n">
@@ -2078,7 +2044,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C41" s="0" t="n">
@@ -2104,7 +2070,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C42" s="0" t="n">
@@ -2130,7 +2096,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C43" s="0" t="n">
@@ -2156,7 +2122,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C44" s="0" t="n">
@@ -2182,7 +2148,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C45" s="0" t="n">
@@ -2208,7 +2174,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C46" s="0" t="n">
@@ -2234,7 +2200,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C47" s="0" t="n">
@@ -2260,7 +2226,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C48" s="0" t="n">
@@ -2286,7 +2252,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C49" s="0" t="n">
@@ -2312,7 +2278,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C50" s="0" t="n">
@@ -2338,7 +2304,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C51" s="0" t="n">
@@ -2364,7 +2330,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C52" s="0" t="n">
@@ -2390,43 +2356,43 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="G53" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="H53" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="I53" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J53" s="3" t="s">
+      <c r="J53" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="K53" s="3" t="s">
+      <c r="K53" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L53" s="3" t="s">
+      <c r="L53" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M53" s="3" t="s">
+      <c r="M53" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N53" s="3" t="s">
+      <c r="N53" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2490,20 +2456,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2553,24 +2519,24 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.62"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2623,7 +2589,7 @@
         <v>98</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
change column name substance unit to emission_unit
</commit_message>
<xml_diff>
--- a/tests/edb/data/areasourceactivities.xlsx
+++ b/tests/edb/data/areasourceactivities.xlsx
@@ -63,7 +63,7 @@
     <t xml:space="preserve">subst:PM10</t>
   </si>
   <si>
-    <t xml:space="preserve">unit</t>
+    <t xml:space="preserve">emission_unit</t>
   </si>
   <si>
     <t xml:space="preserve">act:Residential-plants-Open-fireplaces-wood</t>
@@ -556,10 +556,10 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.09"/>
@@ -790,7 +790,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
   </cols>
@@ -842,7 +842,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
@@ -962,7 +962,7 @@
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2456,7 +2456,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
@@ -2519,7 +2519,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>

</xml_diff>

<commit_message>
assume wkt is wgs84
</commit_message>
<xml_diff>
--- a/tests/edb/data/areasourceactivities.xlsx
+++ b/tests/edb/data/areasourceactivities.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="113">
   <si>
     <t xml:space="preserve">facility_id</t>
   </si>
@@ -39,9 +39,6 @@
     <t xml:space="preserve">geometry</t>
   </si>
   <si>
-    <t xml:space="preserve">EPSG</t>
-  </si>
-  <si>
     <t xml:space="preserve">timevar</t>
   </si>
   <si>
@@ -75,7 +72,7 @@
     <t xml:space="preserve">areasource1</t>
   </si>
   <si>
-    <t xml:space="preserve">POLYGON ((2449702.70275976 5078151.62902639,2450837.61057971 5078021.39370279,2450744.58534857 5077216.7254534,2450102.71125368 5077077.18760669,2449591.07248239 5077249.2842843,2449702.70275976 5078151.62902639))</t>
+    <t xml:space="preserve">POLYGON ((22.006 41.444,22.016 41.443,22.015 41.438,22.009 41.437,22.005 41.438,22.006 41.444))</t>
   </si>
   <si>
     <t xml:space="preserve">1.3</t>
@@ -87,7 +84,7 @@
     <t xml:space="preserve">areasource2</t>
   </si>
   <si>
-    <t xml:space="preserve">POLYGON ((2449418.97580478 5076253.91431107,2449879.45069894 5076691.13289745,2450521.32479382 5076737.64551302,2450814.35427192 5076374.84711156,2450698.072733 5075681.80913954,2449651.53888264 5075328.3132612,2449418.97580478 5076253.91431107))</t>
+    <t xml:space="preserve">POLYGON ((22.003 41.431,22.007 41.434,22.013 41.435,22.016 41.432,22.014 41.428,22.005 41.425,22.003 41.431))</t>
   </si>
   <si>
     <t xml:space="preserve">1-b</t>
@@ -99,7 +96,7 @@
     <t xml:space="preserve">areasource3</t>
   </si>
   <si>
-    <t xml:space="preserve">POLYGON ((2441769.48069413 5078251.37652748,2442293.71664687 5078431.58263624,2442739.3172067 5078185.84703339,2442880.205619 5078212.05883103,2443948.3363727 5076603.30975106,2442788.46432727 5076478.80371229,2441769.48069413 5078251.37652748))</t>
+    <t xml:space="preserve">POLYGON ((21.9347884480412 41.4453304271493,21.9394977397296 41.4465438625105,21.9435006376646 41.4448891723006,21.9447662598059 41.4450656746002,21.9543614416207 41.4342319564415,21.9439421337604 41.4333934262775,21.9347884480412 41.4453304271493))</t>
   </si>
   <si>
     <t xml:space="preserve">officehours</t>
@@ -114,7 +111,7 @@
     <t xml:space="preserve">areasource4</t>
   </si>
   <si>
-    <t xml:space="preserve">POLYGON ((2445081.11344401 5079793.39383044,2447785.96016067 5080725.2070534,2447617.71610652 5077813.29073163,2445301.12489943 5078033.30218706,2445081.11344401 5079793.39383044))</t>
+    <t xml:space="preserve">POLYGON ((21.9645373511873 41.455713016914,21.9888354026551 41.4619862230537,21.987324040602 41.4423804391921,21.9665137477182 41.4438619720198,21.9645373511873 41.455713016914))</t>
   </si>
   <si>
     <t xml:space="preserve">activity_name</t>
@@ -553,20 +550,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="34.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="34.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -606,132 +603,117 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
-        <v>13</v>
-      </c>
+      <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>3857</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="N2" s="0" t="n">
+      <c r="G2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="M2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="O2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>3857</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="0" t="n">
+      <c r="M3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="O3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>3857</v>
-      </c>
       <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>3857</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="N5" s="0" t="n">
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="M5" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
@@ -749,24 +731,22 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -790,34 +770,34 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -842,7 +822,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
@@ -850,33 +830,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>4600</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3" t="str">
         <f aca="false">INDEX(Activity!B:B,MATCH(A2,Activity!A:A,0),1)</f>
@@ -885,16 +865,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>484</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3" t="str">
         <f aca="false">INDEX(Activity!B:B,MATCH(A3,Activity!A:A,0),1)</f>
@@ -903,16 +883,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>900</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3" t="str">
         <f aca="false">INDEX(Activity!B:B,MATCH(A4,Activity!A:A,0),1)</f>
@@ -921,16 +901,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>900</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3" t="str">
         <f aca="false">INDEX(Activity!B:B,MATCH(A5,Activity!A:A,0),1)</f>
@@ -962,43 +942,43 @@
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>100</v>
@@ -1024,7 +1004,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>100</v>
@@ -1050,7 +1030,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>100</v>
@@ -1076,7 +1056,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>100</v>
@@ -1102,7 +1082,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>100</v>
@@ -1128,7 +1108,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>100</v>
@@ -1154,7 +1134,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>100</v>
@@ -1180,7 +1160,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>100</v>
@@ -1206,7 +1186,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>100</v>
@@ -1232,7 +1212,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>100</v>
@@ -1258,7 +1238,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>100</v>
@@ -1284,7 +1264,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>100</v>
@@ -1310,7 +1290,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>100</v>
@@ -1336,7 +1316,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>100</v>
@@ -1362,7 +1342,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>100</v>
@@ -1388,7 +1368,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>100</v>
@@ -1414,7 +1394,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>100</v>
@@ -1440,7 +1420,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>100</v>
@@ -1466,7 +1446,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>100</v>
@@ -1492,7 +1472,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>100</v>
@@ -1518,7 +1498,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>100</v>
@@ -1544,7 +1524,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>100</v>
@@ -1570,7 +1550,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>100</v>
@@ -1596,7 +1576,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>100</v>
@@ -1622,43 +1602,43 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="K26" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="L26" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="M26" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="N26" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1701,39 +1681,39 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>0</v>
@@ -1759,7 +1739,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>0</v>
@@ -1785,7 +1765,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>0</v>
@@ -1811,7 +1791,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>0</v>
@@ -1837,7 +1817,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>0</v>
@@ -1863,7 +1843,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
@@ -1889,7 +1869,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>0</v>
@@ -1915,7 +1895,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>0</v>
@@ -1941,7 +1921,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>0</v>
@@ -1967,7 +1947,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>100</v>
@@ -1993,7 +1973,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>100</v>
@@ -2019,7 +1999,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>100</v>
@@ -2045,7 +2025,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>100</v>
@@ -2071,7 +2051,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>100</v>
@@ -2097,7 +2077,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>100</v>
@@ -2123,7 +2103,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>100</v>
@@ -2149,7 +2129,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>100</v>
@@ -2175,7 +2155,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>0</v>
@@ -2201,7 +2181,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>0</v>
@@ -2227,7 +2207,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>0</v>
@@ -2253,7 +2233,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>0</v>
@@ -2279,7 +2259,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>0</v>
@@ -2305,7 +2285,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>0</v>
@@ -2331,7 +2311,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>0</v>
@@ -2357,43 +2337,43 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="H53" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="I53" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I53" s="2" t="s">
+      <c r="J53" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J53" s="2" t="s">
+      <c r="K53" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="L53" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L53" s="2" t="s">
+      <c r="M53" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M53" s="2" t="s">
+      <c r="N53" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="N53" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2456,7 +2436,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
@@ -2464,37 +2444,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2519,7 +2499,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>
@@ -2528,71 +2508,71 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>